<commit_message>
Finished unit testing for Database class
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46A0B4D-A4E2-4768-BD86-625BCE6DFACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3FCA2B-3261-4D33-937B-25A280D31F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="3" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="700" activeTab="3" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
   <si>
     <t>Test Case</t>
   </si>
@@ -146,9 +146,6 @@
     <t>null query with params</t>
   </si>
   <si>
-    <t>empty query with params</t>
-  </si>
-  <si>
     <t>""</t>
   </si>
   <si>
@@ -170,24 +167,12 @@
     <t>invalid sql query,  params</t>
   </si>
   <si>
-    <t>null query and null params</t>
-  </si>
-  <si>
     <t>valid query with invalid params</t>
   </si>
   <si>
     <t>[1,2,3]</t>
   </si>
   <si>
-    <t>empty query with empty params</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>valid query with empty params</t>
-  </si>
-  <si>
     <t>"foobar"</t>
   </si>
   <si>
@@ -198,6 +183,9 @@
   </si>
   <si>
     <t>PDO Exception</t>
+  </si>
+  <si>
+    <t>empty query without params</t>
   </si>
 </sst>
 </file>
@@ -367,13 +355,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -974,10 +962,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2D8FC6-27F3-48FB-BB89-4D60CA1562E6}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,23 +979,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1035,7 +1023,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
@@ -1055,10 +1043,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -1075,10 +1063,10 @@
         <v>26</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>24</v>
@@ -1095,13 +1083,13 @@
         <v>28</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1112,16 +1100,16 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1132,16 +1120,16 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>29</v>
@@ -1164,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1181,10 +1169,10 @@
         <v>30</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1195,16 +1183,16 @@
         <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1215,76 +1203,16 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update unit testing for database create method
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3FCA2B-3261-4D33-937B-25A280D31F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7576B809-4C41-47F0-B1B2-9559C1E9E02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="700" activeTab="3" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="1" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="47">
   <si>
     <t>Test Case</t>
   </si>
@@ -95,12 +95,6 @@
     <t>PDO Instance</t>
   </si>
   <si>
-    <t>Creates Database</t>
-  </si>
-  <si>
-    <t>No Exceptions (void)</t>
-  </si>
-  <si>
     <t>Prints Success Message</t>
   </si>
   <si>
@@ -186,6 +180,12 @@
   </si>
   <si>
     <t>empty query without params</t>
+  </si>
+  <si>
+    <t>Database doesn't exist</t>
+  </si>
+  <si>
+    <t>Database already exists</t>
   </si>
 </sst>
 </file>
@@ -848,15 +848,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF14DCF-5EB1-41B8-BA03-50477B8EABD9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -889,13 +889,30 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
+        <v>45</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -946,13 +963,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -964,7 +981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2D8FC6-27F3-48FB-BB89-4D60CA1562E6}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1004,10 +1021,10 @@
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
@@ -1017,19 +1034,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1037,19 +1054,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1057,19 +1074,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1077,19 +1094,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1097,19 +1114,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="F7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1117,22 +1134,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1140,19 +1157,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1160,19 +1177,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1180,19 +1197,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1200,19 +1217,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added unit testing for LoginManager methods
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -8,21 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7576B809-4C41-47F0-B1B2-9559C1E9E02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEEACC-B14C-4F64-B48F-E6469AA9A1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="1" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="922" firstSheet="6" activeTab="7" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
     <sheet name="Database Create" sheetId="8" r:id="rId2"/>
     <sheet name="Database CreateSuccessMsg" sheetId="9" r:id="rId3"/>
     <sheet name="Database ProcessQuery" sheetId="10" r:id="rId4"/>
-    <sheet name="Login" sheetId="1" r:id="rId5"/>
-    <sheet name="Logout" sheetId="2" r:id="rId6"/>
-    <sheet name="Registration" sheetId="3" r:id="rId7"/>
-    <sheet name="ChangePassword" sheetId="4" r:id="rId8"/>
-    <sheet name="Auth2" sheetId="5" r:id="rId9"/>
-    <sheet name="Admin" sheetId="6" r:id="rId10"/>
+    <sheet name="LoginManager ProcessLogin" sheetId="11" r:id="rId5"/>
+    <sheet name="LoginManager FailedLogin" sheetId="12" r:id="rId6"/>
+    <sheet name="LoginManager ResetPassword" sheetId="13" r:id="rId7"/>
+    <sheet name="LoginManager IsLockedOut" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="98">
   <si>
     <t>Test Case</t>
   </si>
@@ -65,12 +63,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
     <t>Valid</t>
   </si>
   <si>
@@ -86,9 +78,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>PDO Object</t>
-  </si>
-  <si>
     <t>PDOException</t>
   </si>
   <si>
@@ -186,6 +175,168 @@
   </si>
   <si>
     <t>Database already exists</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>ipAddr</t>
+  </si>
+  <si>
+    <t>invalid uid and pwd</t>
+  </si>
+  <si>
+    <t>valid uid, invalid pwd</t>
+  </si>
+  <si>
+    <t>valid uid, pwd</t>
+  </si>
+  <si>
+    <t>valid uid, empty pwd</t>
+  </si>
+  <si>
+    <t>empty uid, empty pwd</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>Password1!</t>
+  </si>
+  <si>
+    <t>GetIpAddress()</t>
+  </si>
+  <si>
+    <t>foobar</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>invalid uid, empty pwd</t>
+  </si>
+  <si>
+    <t>empty uid, invalid pwd</t>
+  </si>
+  <si>
+    <t>valid uid, null pwd</t>
+  </si>
+  <si>
+    <t>null uid, valid pwd</t>
+  </si>
+  <si>
+    <t>SQLi payload</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>password' OR '1'='1' --</t>
+  </si>
+  <si>
+    <t>SQLi payload test</t>
+  </si>
+  <si>
+    <t>valid uid and ipAddr</t>
+  </si>
+  <si>
+    <t>GeIpAddress()</t>
+  </si>
+  <si>
+    <t>null uid, valid ipAddr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid </t>
+  </si>
+  <si>
+    <t>empty uid, valid ipAddr</t>
+  </si>
+  <si>
+    <t>newpass</t>
+  </si>
+  <si>
+    <t>oldpass</t>
+  </si>
+  <si>
+    <t>newConfirm</t>
+  </si>
+  <si>
+    <t>all valid inputs</t>
+  </si>
+  <si>
+    <t>Password2!</t>
+  </si>
+  <si>
+    <t>mismatch new password</t>
+  </si>
+  <si>
+    <t>invalid old password</t>
+  </si>
+  <si>
+    <t>Password3!</t>
+  </si>
+  <si>
+    <t>Password10!</t>
+  </si>
+  <si>
+    <t>new pass less than 8 chars</t>
+  </si>
+  <si>
+    <t>invalid uid</t>
+  </si>
+  <si>
+    <t>userOne</t>
+  </si>
+  <si>
+    <t>Word2!</t>
+  </si>
+  <si>
+    <t>new pass no uppercase</t>
+  </si>
+  <si>
+    <t>password2!</t>
+  </si>
+  <si>
+    <t>new pass no digits</t>
+  </si>
+  <si>
+    <t>Password!!</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>loginCount</t>
+  </si>
+  <si>
+    <t>testIP</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>has never logged in before</t>
+  </si>
+  <si>
+    <t>has failed 5 attempts</t>
+  </si>
+  <si>
+    <t>has failed 4 attempts</t>
+  </si>
+  <si>
+    <t>has failed 1 attempt</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>null uid</t>
   </si>
 </sst>
 </file>
@@ -209,13 +360,14 @@
     </font>
     <font>
       <i/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -231,27 +383,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -271,33 +408,7 @@
       <left style="medium">
         <color rgb="FFCCCCCC"/>
       </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
       <right/>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
       <top style="medium">
         <color rgb="FFCCCCCC"/>
       </top>
@@ -328,59 +439,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,7 +820,7 @@
     <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -755,16 +845,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -772,76 +862,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6A573F-0C25-45C5-996C-B0109D28903D}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -850,7 +883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF14DCF-5EB1-41B8-BA03-50477B8EABD9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -886,13 +919,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -903,13 +936,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -925,7 +958,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,7 +978,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -960,16 +993,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -981,72 +1014,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2D8FC6-27F3-48FB-BB89-4D60CA1562E6}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>12</v>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1054,19 +1087,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>34</v>
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1074,19 +1107,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1094,19 +1127,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,19 +1147,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
         <v>40</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1134,22 +1167,22 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>27</v>
+        <v>40</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1157,19 +1190,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>12</v>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1177,19 +1210,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>39</v>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1197,19 +1230,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>12</v>
+        <v>41</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1217,19 +1250,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1247,130 +1280,424 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F56B6-00BD-4254-8A55-8196DD1212E4}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A5059A-C94D-4663-B193-68CF554C4A0A}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C08B590-56A7-4A6D-BC40-CD260C7EF926}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C321EB0-E1D4-442E-B345-7BF49F6CA98D}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="3"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="14"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
@@ -1379,171 +1706,454 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DD9F26-13CD-4F24-9311-312B0105116F}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2864E955-D665-4F39-A1EB-7FEC70CF1B68}">
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="14"/>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="D1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDFDE82-C086-4DD5-953A-CAFDB40CB8C6}">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA6E850-92F0-43CC-AC98-4B227E8DB052}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="14"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8FDC4F-EB20-41D0-9731-675E4B2B62B4}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="14"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added unit testing for LoginManager ProcessRegistration
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAEEACC-B14C-4F64-B48F-E6469AA9A1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A8787-65FF-4863-B117-C6CBB3BEB347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="922" firstSheet="6" activeTab="7" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="933" firstSheet="4" activeTab="9" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="LoginManager FailedLogin" sheetId="12" r:id="rId6"/>
     <sheet name="LoginManager ResetPassword" sheetId="13" r:id="rId7"/>
     <sheet name="LoginManager IsLockedOut" sheetId="14" r:id="rId8"/>
+    <sheet name="LoginManager ProcessRegistratio" sheetId="15" r:id="rId9"/>
+    <sheet name="LoginManager FailedRegistration" sheetId="16" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="107">
   <si>
     <t>Test Case</t>
   </si>
@@ -337,6 +339,33 @@
   </si>
   <si>
     <t>null uid</t>
+  </si>
+  <si>
+    <t>userTwo</t>
+  </si>
+  <si>
+    <t>GetIPAddress()</t>
+  </si>
+  <si>
+    <t>invalid uid format</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>invalid pwd format</t>
+  </si>
+  <si>
+    <t>passwordTwo</t>
+  </si>
+  <si>
+    <t>empty uid</t>
+  </si>
+  <si>
+    <t>empty pwd</t>
+  </si>
+  <si>
+    <t>null pwd</t>
   </si>
 </sst>
 </file>
@@ -466,11 +495,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -879,6 +908,67 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6EFF6B-A3C3-4BB8-8E1E-B3BC27001382}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF14DCF-5EB1-41B8-BA03-50477B8EABD9}">
   <dimension ref="A1:F3"/>
@@ -1298,10 +1388,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -1310,8 +1400,8 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1320,8 +1410,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="8"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
@@ -1332,8 +1422,8 @@
       <c r="F2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1599,10 +1689,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -1611,7 +1701,7 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
+      <c r="E1" s="8"/>
       <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1620,8 +1710,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="8"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
@@ -1629,8 +1719,8 @@
       <c r="E2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1723,10 +1813,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -1735,9 +1825,9 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1746,8 +1836,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="8"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
@@ -1761,8 +1851,8 @@
       <c r="G2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1963,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA6E850-92F0-43CC-AC98-4B227E8DB052}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1975,10 +2065,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
@@ -1987,9 +2077,9 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
       <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
@@ -1998,8 +2088,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="8"/>
       <c r="D2" s="6" t="s">
         <v>46</v>
@@ -2013,8 +2103,8 @@
       <c r="G2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2144,6 +2234,236 @@
       </c>
       <c r="H7" t="s">
         <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="H1:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35E5323-C7E6-4523-815B-ADF166D56337}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2151,9 +2471,9 @@
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added unit testing for LoginManager FailedRegistration
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580A8787-65FF-4863-B117-C6CBB3BEB347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B100D2-C0C7-4D79-825C-379F1DB43595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="933" firstSheet="4" activeTab="9" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="933" firstSheet="4" activeTab="9" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="109">
   <si>
     <t>Test Case</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>null pwd</t>
+  </si>
+  <si>
+    <t>already existing uid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid uid </t>
   </si>
 </sst>
 </file>
@@ -468,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -500,6 +506,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -910,15 +919,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6EFF6B-A3C3-4BB8-8E1E-B3BC27001382}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -932,38 +946,134 @@
         <v>3</v>
       </c>
       <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="G1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="8"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="D1:E1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1676,7 +1786,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F3" sqref="B3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2280,8 +2390,8 @@
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
@@ -2302,7 +2412,7 @@
       <c r="F2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="11"/>
+      <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Implemented LoginManager into main app
</commit_message>
<xml_diff>
--- a/tests/BlackBox_TestCases.xlsx
+++ b/tests/BlackBox_TestCases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project 24\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B100D2-C0C7-4D79-825C-379F1DB43595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260A5B9-4205-45BE-BEF8-CB7F60B6CD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" tabRatio="933" firstSheet="4" activeTab="9" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="933" firstSheet="2" activeTab="7" xr2:uid="{3D83DA18-7D1C-46CD-AE11-304C67514BDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Database GetConnection" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="108">
   <si>
     <t>Test Case</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>has failed 1 attempt</t>
-  </si>
-  <si>
-    <t>Exception</t>
   </si>
   <si>
     <t>null uid</t>
@@ -474,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -492,6 +489,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -502,12 +502,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -921,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6EFF6B-A3C3-4BB8-8E1E-B3BC27001382}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -933,41 +927,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="12">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -977,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
         <v>67</v>
@@ -987,14 +981,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>52</v>
@@ -1007,17 +1001,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>67</v>
@@ -1027,7 +1021,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1047,7 +1041,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1229,38 +1223,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1498,31 +1492,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1532,8 +1526,8 @@
       <c r="F2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1799,38 +1793,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -1923,32 +1917,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
@@ -1961,8 +1955,8 @@
       <c r="G2" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -2163,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA6E850-92F0-43CC-AC98-4B227E8DB052}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2175,32 +2169,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>46</v>
       </c>
@@ -2213,8 +2207,8 @@
       <c r="G2" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2328,7 +2322,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" t="s">
         <v>90</v>
@@ -2342,8 +2336,8 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" t="s">
-        <v>96</v>
+      <c r="H7" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2378,31 +2372,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
@@ -2412,8 +2406,8 @@
       <c r="F2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2426,13 +2420,13 @@
         <v>74</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -2446,16 +2440,16 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
         <v>100</v>
-      </c>
-      <c r="D4" t="s">
-        <v>101</v>
       </c>
       <c r="E4" t="s">
         <v>75</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -2469,16 +2463,16 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
         <v>102</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>98</v>
-      </c>
-      <c r="E5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s">
-        <v>99</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -2492,7 +2486,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
         <v>28</v>
@@ -2501,7 +2495,7 @@
         <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -2515,16 +2509,16 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -2538,7 +2532,7 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
         <v>25</v>
@@ -2547,7 +2541,7 @@
         <v>75</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -2561,16 +2555,16 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>

</xml_diff>